<commit_message>
Fine presa dati e continuo analisi
</commit_message>
<xml_diff>
--- a/Circuiti3/dati_rl.xlsx
+++ b/Circuiti3/dati_rl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ALL\Stefano\Bicocca\secondo_anno\lab2\Laboratorio_2\Circuiti3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEA061C-9A78-401D-8BE7-420E387AD2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98917453-F393-48A0-9C75-F3F5C3AA7B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,661 +397,721 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="B2">
-        <v>9.6</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>9.0399999999999991</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D2">
-        <v>1.36</v>
+        <v>0.4</v>
       </c>
       <c r="E2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>-68</v>
+        <v>-84</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>700</v>
+        <v>250</v>
       </c>
       <c r="B3">
-        <v>9.6</v>
+        <v>9.9</v>
       </c>
       <c r="C3">
-        <v>9.0399999999999991</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D3">
-        <v>1.84</v>
+        <v>0.7</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>-69</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>900</v>
+        <v>400</v>
       </c>
       <c r="B4">
-        <v>9.6</v>
+        <v>9.9</v>
       </c>
       <c r="C4">
-        <v>8.9</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D4">
-        <v>2.2000000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>-63</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1100</v>
+        <v>500</v>
       </c>
       <c r="B5">
         <v>9.6</v>
       </c>
       <c r="C5">
-        <v>8.8000000000000007</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="D5">
-        <v>2.64</v>
+        <v>1.36</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F5">
-        <v>-62</v>
+        <v>-68</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1400</v>
+        <v>700</v>
       </c>
       <c r="B6">
         <v>9.6</v>
       </c>
       <c r="C6">
-        <v>8.6999999999999993</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="D6">
-        <v>3.04</v>
+        <v>1.84</v>
       </c>
       <c r="E6">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>-66</v>
+        <v>-69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1700</v>
+        <v>900</v>
       </c>
       <c r="B7">
-        <v>9.6999999999999993</v>
+        <v>9.6</v>
       </c>
       <c r="C7">
-        <v>8.4</v>
+        <v>8.9</v>
       </c>
       <c r="D7">
-        <v>3.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E7">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>-62</v>
+        <v>-63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2000</v>
+        <v>1100</v>
       </c>
       <c r="B8">
-        <v>9.76</v>
+        <v>9.6</v>
       </c>
       <c r="C8">
-        <v>8.32</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D8">
-        <v>4.24</v>
+        <v>2.64</v>
       </c>
       <c r="E8">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>-60</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2200</v>
+        <v>1400</v>
       </c>
       <c r="B9">
-        <v>9.76</v>
+        <v>9.6</v>
       </c>
       <c r="C9">
-        <v>8.1</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D9">
-        <v>4.5599999999999996</v>
+        <v>3.04</v>
       </c>
       <c r="E9">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F9">
-        <v>-58</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2400</v>
+        <v>1700</v>
       </c>
       <c r="B10">
-        <v>9.76</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="D10">
-        <v>4.88</v>
+        <v>3.6</v>
       </c>
       <c r="E10">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F10">
-        <v>-56</v>
+        <v>-62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2600</v>
+        <v>2000</v>
       </c>
       <c r="B11">
         <v>9.76</v>
       </c>
       <c r="C11">
-        <v>7.76</v>
+        <v>8.32</v>
       </c>
       <c r="D11">
-        <v>5.2</v>
+        <v>4.24</v>
       </c>
       <c r="E11">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F11">
-        <v>-51</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2700</v>
+        <v>2200</v>
       </c>
       <c r="B12">
         <v>9.76</v>
       </c>
       <c r="C12">
-        <v>7.68</v>
+        <v>8.1</v>
       </c>
       <c r="D12">
-        <v>5.36</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="E12">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F12">
-        <v>-51</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2800</v>
+        <v>2400</v>
       </c>
       <c r="B13">
         <v>9.76</v>
       </c>
       <c r="C13">
-        <v>7.68</v>
+        <v>8</v>
       </c>
       <c r="D13">
-        <v>5.52</v>
+        <v>4.88</v>
       </c>
       <c r="E13">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F13">
-        <v>-50</v>
+        <v>-56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2900</v>
+        <v>2600</v>
       </c>
       <c r="B14">
         <v>9.76</v>
       </c>
       <c r="C14">
-        <v>7.5</v>
+        <v>7.76</v>
       </c>
       <c r="D14">
-        <v>5.68</v>
+        <v>5.2</v>
       </c>
       <c r="E14">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F14">
-        <v>-49</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3000</v>
+        <v>2700</v>
       </c>
       <c r="B15">
         <v>9.76</v>
       </c>
       <c r="C15">
-        <v>7.44</v>
+        <v>7.68</v>
       </c>
       <c r="D15">
-        <v>5.84</v>
+        <v>5.36</v>
       </c>
       <c r="E15">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15">
-        <v>-48</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3100</v>
+        <v>2800</v>
       </c>
       <c r="B16">
         <v>9.76</v>
       </c>
       <c r="C16">
-        <v>7.36</v>
+        <v>7.68</v>
       </c>
       <c r="D16">
-        <v>5.92</v>
+        <v>5.52</v>
       </c>
       <c r="E16">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F16">
-        <v>-47</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3200</v>
+        <v>2900</v>
       </c>
       <c r="B17">
         <v>9.76</v>
       </c>
       <c r="C17">
-        <v>7.28</v>
+        <v>7.5</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>5.68</v>
       </c>
       <c r="E17">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17">
-        <v>-47</v>
+        <v>-49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3300</v>
+        <v>3000</v>
       </c>
       <c r="B18">
         <v>9.76</v>
       </c>
       <c r="C18">
-        <v>7.2</v>
+        <v>7.44</v>
       </c>
       <c r="D18">
-        <v>6.16</v>
+        <v>5.84</v>
       </c>
       <c r="E18">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F18">
-        <v>-46</v>
+        <v>-48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3400</v>
+        <v>3100</v>
       </c>
       <c r="B19">
         <v>9.76</v>
       </c>
       <c r="C19">
-        <v>7.12</v>
+        <v>7.36</v>
       </c>
       <c r="D19">
-        <v>6.3</v>
+        <v>5.92</v>
       </c>
       <c r="E19">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F19">
-        <v>-46</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>3500</v>
+        <v>3200</v>
       </c>
       <c r="B20">
         <v>9.76</v>
       </c>
       <c r="C20">
-        <v>7.04</v>
+        <v>7.28</v>
       </c>
       <c r="D20">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="E20">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F20">
-        <v>-45</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>3700</v>
+        <v>3300</v>
       </c>
       <c r="B21">
         <v>9.76</v>
       </c>
       <c r="C21">
-        <v>6.88</v>
+        <v>7.2</v>
       </c>
       <c r="D21">
-        <v>6.64</v>
+        <v>6.16</v>
       </c>
       <c r="E21">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F21">
-        <v>-45</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>4000</v>
+        <v>3400</v>
       </c>
       <c r="B22">
-        <v>9.84</v>
+        <v>9.76</v>
       </c>
       <c r="C22">
-        <v>6.64</v>
+        <v>7.12</v>
       </c>
       <c r="D22">
-        <v>6.88</v>
+        <v>6.3</v>
       </c>
       <c r="E22">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F22">
-        <v>-42</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>4500</v>
+        <v>3500</v>
       </c>
       <c r="B23">
-        <v>9.92</v>
+        <v>9.76</v>
       </c>
       <c r="C23">
-        <v>6.24</v>
+        <v>7.04</v>
       </c>
       <c r="D23">
-        <v>7.28</v>
+        <v>6.4</v>
       </c>
       <c r="E23">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F23">
-        <v>-38</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>5000</v>
+        <v>3700</v>
       </c>
       <c r="B24">
-        <v>9.92</v>
+        <v>9.76</v>
       </c>
       <c r="C24">
-        <v>5.84</v>
+        <v>6.88</v>
       </c>
       <c r="D24">
-        <v>7.68</v>
+        <v>6.64</v>
       </c>
       <c r="E24">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F24">
-        <v>-36</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="B25">
-        <v>9.92</v>
+        <v>9.84</v>
       </c>
       <c r="C25">
-        <v>5.2</v>
+        <v>6.64</v>
       </c>
       <c r="D25">
-        <v>8.16</v>
+        <v>6.88</v>
       </c>
       <c r="E25">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F25">
-        <v>-31</v>
+        <v>-42</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>7000</v>
+        <v>4500</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>9.92</v>
       </c>
       <c r="C26">
-        <v>4.6399999999999997</v>
+        <v>6.24</v>
       </c>
       <c r="D26">
-        <v>8.56</v>
+        <v>7.28</v>
       </c>
       <c r="E26">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F26">
-        <v>-28</v>
+        <v>-38</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>9.92</v>
       </c>
       <c r="C27">
-        <v>4.24</v>
+        <v>5.84</v>
       </c>
       <c r="D27">
-        <v>8.8000000000000007</v>
+        <v>7.68</v>
       </c>
       <c r="E27">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F27">
-        <v>-25</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>9.92</v>
       </c>
       <c r="C28">
-        <v>3.6</v>
+        <v>5.2</v>
       </c>
       <c r="D28">
-        <v>9.1199999999999992</v>
+        <v>8.16</v>
       </c>
       <c r="E28">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F28">
-        <v>-20</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>15000</v>
+        <v>7000</v>
       </c>
       <c r="B29">
-        <v>10.08</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>2.48</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="D29">
-        <v>9.6</v>
+        <v>8.56</v>
       </c>
       <c r="E29">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F29">
-        <v>-14</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>20000</v>
+        <v>8000</v>
       </c>
       <c r="B30">
-        <v>10.08</v>
+        <v>10</v>
       </c>
       <c r="C30">
-        <v>1.8</v>
+        <v>4.24</v>
       </c>
       <c r="D30">
-        <v>9.4</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E30">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F30">
-        <v>-9</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="B31">
-        <v>10.199999999999999</v>
+        <v>10</v>
       </c>
       <c r="C31">
-        <v>1.28</v>
+        <v>3.6</v>
       </c>
       <c r="D31">
-        <v>9.6</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="E31">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F31">
-        <v>-9</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>50000</v>
+        <v>15000</v>
       </c>
       <c r="B32">
-        <v>10.4</v>
+        <v>10.08</v>
       </c>
       <c r="C32">
-        <v>0.8</v>
+        <v>2.48</v>
       </c>
       <c r="D32">
         <v>9.6</v>
       </c>
       <c r="E32">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F32">
-        <v>-6</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>75000</v>
+        <v>20000</v>
       </c>
       <c r="B33">
-        <v>10.4</v>
+        <v>10.08</v>
       </c>
       <c r="C33">
-        <v>0.48</v>
+        <v>1.8</v>
       </c>
       <c r="D33">
-        <v>9.8000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="E33">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F33">
-        <v>-2</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
+        <v>30000</v>
+      </c>
+      <c r="B34">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C34">
+        <v>1.28</v>
+      </c>
+      <c r="D34">
+        <v>9.6</v>
+      </c>
+      <c r="E34">
+        <v>83</v>
+      </c>
+      <c r="F34">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>50000</v>
+      </c>
+      <c r="B35">
+        <v>10.4</v>
+      </c>
+      <c r="C35">
+        <v>0.8</v>
+      </c>
+      <c r="D35">
+        <v>9.6</v>
+      </c>
+      <c r="E35">
+        <v>85</v>
+      </c>
+      <c r="F35">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>75000</v>
+      </c>
+      <c r="B36">
+        <v>10.4</v>
+      </c>
+      <c r="C36">
+        <v>0.48</v>
+      </c>
+      <c r="D36">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E36">
+        <v>89</v>
+      </c>
+      <c r="F36">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>100000</v>
       </c>
-      <c r="B34">
+      <c r="B37">
         <v>10.4</v>
       </c>
-      <c r="C34">
+      <c r="C37">
         <v>0.34</v>
       </c>
-      <c r="D34">
+      <c r="D37">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E34">
+      <c r="E37">
         <v>89</v>
       </c>
-      <c r="F34">
+      <c r="F37">
         <v>-0.5</v>
       </c>
     </row>

</xml_diff>